<commit_message>
Still the same but update pid values
</commit_message>
<xml_diff>
--- a/ExperimentalData/ImpulseResponse_SmallMotor.xlsx
+++ b/ExperimentalData/ImpulseResponse_SmallMotor.xlsx
@@ -114,7 +114,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2456,11 +2455,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="457468000"/>
-        <c:axId val="457462904"/>
+        <c:axId val="480666552"/>
+        <c:axId val="480667336"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="457468000"/>
+        <c:axId val="480666552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2517,12 +2516,12 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="457462904"/>
+        <c:crossAx val="480667336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="457462904"/>
+        <c:axId val="480667336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2579,7 +2578,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="457468000"/>
+        <c:crossAx val="480666552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2593,7 +2592,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -15855,11 +15853,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="197666920"/>
-        <c:axId val="197661824"/>
+        <c:axId val="480668904"/>
+        <c:axId val="480667728"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="197666920"/>
+        <c:axId val="480668904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15977,12 +15975,12 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="197661824"/>
+        <c:crossAx val="480667728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="197661824"/>
+        <c:axId val="480667728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16100,7 +16098,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="197666920"/>
+        <c:crossAx val="480668904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -17300,14 +17298,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>219074</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>161926</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>152399</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
+      <xdr:colOff>466726</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>152399</xdr:rowOff>
     </xdr:to>

</xml_diff>